<commit_message>
menambahkan data kost dan revisi pertama dari pembimbing 1
</commit_message>
<xml_diff>
--- a/Excel/STUDI KASUS.xlsx
+++ b/Excel/STUDI KASUS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNDIPA\Semester 7\Skripsi\skripsi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KULIAH\SEMESTER 7\PROPOSAL SKRIPSI\skripsi\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54368FA-0DB4-4E6B-8869-E721CF92759E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7AD738-62BC-47DC-A182-C5680BEE615D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="691" activeTab="3" xr2:uid="{901D0503-6946-40CA-8D36-37B156763246}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="691" xr2:uid="{901D0503-6946-40CA-8D36-37B156763246}"/>
   </bookViews>
   <sheets>
     <sheet name="Kost" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1789" uniqueCount="497">
   <si>
     <t xml:space="preserve">Biaya </t>
   </si>
@@ -1444,6 +1444,135 @@
   </si>
   <si>
     <t>bulanan</t>
+  </si>
+  <si>
+    <t>Pondok Virda</t>
+  </si>
+  <si>
+    <t>Jalan Sahabat 6</t>
+  </si>
+  <si>
+    <t>Putri/Putra</t>
+  </si>
+  <si>
+    <t>CCTV sama penjaga</t>
+  </si>
+  <si>
+    <t>pemilk = Akil, narasumber = irfan</t>
+  </si>
+  <si>
+    <t>085323455503 = akil</t>
+  </si>
+  <si>
+    <t>ibu susan</t>
+  </si>
+  <si>
+    <t>Pondok Azizah</t>
+  </si>
+  <si>
+    <t>Jalan Sahabat 5</t>
+  </si>
+  <si>
+    <t>Rp. 9.000.000 per tahun</t>
+  </si>
+  <si>
+    <t>Rp. 7.500.000 per tahun</t>
+  </si>
+  <si>
+    <t>lemari, spring bed, wc dalam, rak penyimpanan alat masak, AC, parkir</t>
+  </si>
+  <si>
+    <t>Perbulan dan sumur bor</t>
+  </si>
+  <si>
+    <t>23,00</t>
+  </si>
+  <si>
+    <t>Pondok Yumma</t>
+  </si>
+  <si>
+    <t>Akbar</t>
+  </si>
+  <si>
+    <t>Rp. 8.500.000 per tahun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perbulan </t>
+  </si>
+  <si>
+    <t>tidak ada batas jam malam</t>
+  </si>
+  <si>
+    <t>0812 9898 1575</t>
+  </si>
+  <si>
+    <t>Pondok PG ONE</t>
+  </si>
+  <si>
+    <t>Anis Adrian</t>
+  </si>
+  <si>
+    <t>08124255730</t>
+  </si>
+  <si>
+    <t>Jalan sahabt 6 no 5</t>
+  </si>
+  <si>
+    <t>Rp. 7.000.000 per tahun</t>
+  </si>
+  <si>
+    <t>Kasur, lemari, meja, kipas, parkir</t>
+  </si>
+  <si>
+    <t>wc dalam,  lemari, kipas, tempat tidur, parkir</t>
+  </si>
+  <si>
+    <t>Tempat tidur,  lemari, wc dalam, parkir</t>
+  </si>
+  <si>
+    <t>3 x 5</t>
+  </si>
+  <si>
+    <t>diberi kunci</t>
+  </si>
+  <si>
+    <t>Fajarnur</t>
+  </si>
+  <si>
+    <t>Jalan sahabat 6 no 6</t>
+  </si>
+  <si>
+    <t>Rp. 730.000 per bulan</t>
+  </si>
+  <si>
+    <t>Kipas angin , lemari, tempat tidur, wc dalam, parkir</t>
+  </si>
+  <si>
+    <t>Pembayaran Awal</t>
+  </si>
+  <si>
+    <t>pemilik = saipul, narasumber = Ernawati</t>
+  </si>
+  <si>
+    <t>Ernawati=083852260303</t>
+  </si>
+  <si>
+    <t>Pondok Ananda 2</t>
+  </si>
+  <si>
+    <t>sadli</t>
+  </si>
+  <si>
+    <t>Jalan sahabat 6</t>
+  </si>
+  <si>
+    <t>085256608655</t>
+  </si>
+  <si>
+    <t>Rp. 8.000.000 per tahun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spring bed, Lemari, kipas, wc dalam, parkir              </t>
   </si>
 </sst>
 </file>
@@ -2805,30 +2934,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E46AEE5-C1DF-4E3B-B1A0-CC373A6F6C73}">
   <dimension ref="A2:P49"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="76" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="4.44140625" customWidth="1"/>
-    <col min="3" max="3" width="28.21875" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="25.109375" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" customWidth="1"/>
-    <col min="10" max="10" width="13.77734375" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" customWidth="1"/>
-    <col min="14" max="14" width="18.88671875" customWidth="1"/>
-    <col min="15" max="15" width="20.6640625" customWidth="1"/>
-    <col min="16" max="16" width="18.21875" customWidth="1"/>
+    <col min="1" max="2" width="4.453125" customWidth="1"/>
+    <col min="3" max="3" width="28.1796875" customWidth="1"/>
+    <col min="4" max="4" width="17.36328125" customWidth="1"/>
+    <col min="5" max="5" width="25.08984375" customWidth="1"/>
+    <col min="6" max="6" width="18.36328125" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" customWidth="1"/>
+    <col min="8" max="8" width="29" customWidth="1"/>
+    <col min="9" max="9" width="16.08984375" customWidth="1"/>
+    <col min="10" max="10" width="13.81640625" customWidth="1"/>
+    <col min="11" max="11" width="18.08984375" customWidth="1"/>
+    <col min="12" max="12" width="13.453125" customWidth="1"/>
+    <col min="13" max="13" width="11.453125" customWidth="1"/>
+    <col min="14" max="14" width="18.90625" customWidth="1"/>
+    <col min="15" max="15" width="20.6328125" customWidth="1"/>
+    <col min="16" max="16" width="18.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>77</v>
       </c>
@@ -2878,7 +3007,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -2925,7 +3054,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="116" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -2972,7 +3101,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="116" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -3019,7 +3148,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -3069,7 +3198,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -3119,7 +3248,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -3169,7 +3298,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <v>7</v>
       </c>
@@ -3219,7 +3348,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -3265,7 +3394,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -3315,7 +3444,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>10</v>
       </c>
@@ -3365,147 +3494,373 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="9"/>
-      <c r="F13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="9"/>
+    <row r="13" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="9">
+        <v>11</v>
+      </c>
+      <c r="B13" s="9">
+        <v>11</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>458</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="9">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9">
+        <v>12</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>461</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>462</v>
+      </c>
       <c r="F14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B15" s="9"/>
-      <c r="F15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="9"/>
-      <c r="F16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="9"/>
-      <c r="F17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="9"/>
-      <c r="F18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="G14" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="9">
+        <v>13</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="O15" s="9" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="9">
+        <v>14</v>
+      </c>
+      <c r="B16" s="9">
+        <v>14</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>474</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" s="9">
+        <v>15</v>
+      </c>
+      <c r="B17" s="9">
+        <v>15</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>484</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>485</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="O17" s="9" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="9">
+        <v>16</v>
+      </c>
+      <c r="B18" s="9">
+        <v>16</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B19" s="9"/>
       <c r="F19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B20" s="9"/>
       <c r="F20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B21" s="9"/>
       <c r="F21" s="2"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B22" s="9"/>
       <c r="F22" s="2"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B23" s="9"/>
       <c r="F23" s="2"/>
       <c r="N23" s="28"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B24" s="9"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B25" s="9"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B26" s="9"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B27" s="9"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B28" s="9"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B29" s="9"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B30" s="9"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B31" s="9"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B32" s="9"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="9"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="9"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" s="9"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" s="9"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" s="9"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" s="9"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" s="9"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40" s="9"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41" s="9"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42" s="9"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B43" s="9"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44" s="9"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B45" s="9"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B46" s="9"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B47" s="9"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B48" s="9"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B49" s="9"/>
     </row>
   </sheetData>
@@ -3518,31 +3873,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{015FA8AF-97B1-4BAE-BA56-FF4AAB7B8C3B}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.21875" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" customWidth="1"/>
+    <col min="3" max="3" width="16.08984375" customWidth="1"/>
+    <col min="4" max="4" width="24.6328125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" customWidth="1"/>
-    <col min="8" max="8" width="16.21875" customWidth="1"/>
-    <col min="9" max="9" width="23.6640625" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="11" max="11" width="21.88671875" customWidth="1"/>
-    <col min="12" max="12" width="27.44140625" customWidth="1"/>
-    <col min="13" max="13" width="20.21875" customWidth="1"/>
-    <col min="14" max="14" width="22.6640625" customWidth="1"/>
-    <col min="15" max="15" width="16.21875" customWidth="1"/>
-    <col min="16" max="16" width="15.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" customWidth="1"/>
+    <col min="8" max="8" width="16.1796875" customWidth="1"/>
+    <col min="9" max="9" width="23.6328125" customWidth="1"/>
+    <col min="10" max="10" width="14.6328125" customWidth="1"/>
+    <col min="11" max="11" width="21.90625" customWidth="1"/>
+    <col min="12" max="12" width="27.453125" customWidth="1"/>
+    <col min="13" max="13" width="20.1796875" customWidth="1"/>
+    <col min="14" max="14" width="22.6328125" customWidth="1"/>
+    <col min="15" max="15" width="16.1796875" customWidth="1"/>
+    <col min="16" max="16" width="15.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>149</v>
       </c>
@@ -3592,7 +3947,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>168</v>
       </c>
@@ -3640,7 +3995,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>169</v>
       </c>
@@ -3688,7 +4043,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>170</v>
       </c>
@@ -3736,7 +4091,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>223</v>
       </c>
@@ -3786,7 +4141,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>229</v>
       </c>
@@ -3836,7 +4191,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>234</v>
       </c>
@@ -3886,7 +4241,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>353</v>
       </c>
@@ -3936,7 +4291,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>356</v>
       </c>
@@ -3986,7 +4341,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>358</v>
       </c>
@@ -4036,7 +4391,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>359</v>
       </c>
@@ -4080,7 +4435,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>416</v>
       </c>
@@ -4104,22 +4459,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB87EEF9-7F2E-4545-9951-0F532151B120}">
   <dimension ref="A1:V27"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="117" workbookViewId="0">
+    <sheetView zoomScale="117" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.81640625" customWidth="1"/>
     <col min="3" max="4" width="25" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="15" max="15" width="18.77734375" customWidth="1"/>
+    <col min="15" max="15" width="18.81640625" customWidth="1"/>
     <col min="19" max="19" width="15" customWidth="1"/>
-    <col min="22" max="22" width="19.88671875" customWidth="1"/>
+    <col min="22" max="22" width="19.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -4139,7 +4494,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4158,7 +4513,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -4192,7 +4547,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -4226,7 +4581,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -4260,7 +4615,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -4294,7 +4649,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -4325,7 +4680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>324</v>
       </c>
@@ -4359,7 +4714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -4393,7 +4748,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -4409,7 +4764,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>327</v>
       </c>
@@ -4449,7 +4804,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B12">
         <f>Ressponden!B12</f>
         <v>100</v>
@@ -4482,7 +4837,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="G13" t="s">
         <v>140</v>
       </c>
@@ -4511,7 +4866,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="G14" t="s">
         <v>180</v>
       </c>
@@ -4540,7 +4895,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="G15" t="s">
         <v>181</v>
       </c>
@@ -4569,7 +4924,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -4598,7 +4953,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -4624,7 +4979,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -4644,7 +4999,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -4661,7 +5016,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -4678,7 +5033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -4707,7 +5062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -4736,7 +5091,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -4759,7 +5114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -4782,7 +5137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -4805,7 +5160,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -4828,7 +5183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>324</v>
       </c>
@@ -4861,28 +5216,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BA1C62-8752-4999-BB16-F79297149C3E}">
   <dimension ref="A1:P142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="110" zoomScaleNormal="121" workbookViewId="0">
+    <sheetView topLeftCell="A67" zoomScale="79" zoomScaleNormal="121" workbookViewId="0">
       <selection activeCell="F133" sqref="F133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
-    <col min="3" max="4" width="10.21875" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="7" max="7" width="27.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" customWidth="1"/>
-    <col min="11" max="11" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.6328125" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="3" max="4" width="10.1796875" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" customWidth="1"/>
+    <col min="7" max="7" width="27.453125" customWidth="1"/>
+    <col min="8" max="8" width="10.54296875" customWidth="1"/>
+    <col min="9" max="9" width="11.08984375" customWidth="1"/>
+    <col min="10" max="10" width="14.453125" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" customWidth="1"/>
-    <col min="15" max="15" width="20.21875" customWidth="1"/>
-    <col min="19" max="19" width="17.44140625" customWidth="1"/>
+    <col min="13" max="13" width="11.453125" customWidth="1"/>
+    <col min="15" max="15" width="20.1796875" customWidth="1"/>
+    <col min="19" max="19" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>151</v>
       </c>
@@ -4890,7 +5245,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
         <v>152</v>
       </c>
@@ -4898,7 +5253,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="9" t="s">
         <v>19</v>
       </c>
@@ -4924,7 +5279,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="9" t="s">
         <v>20</v>
       </c>
@@ -4950,7 +5305,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="9" t="s">
         <v>21</v>
       </c>
@@ -4976,7 +5331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="9" t="s">
         <v>22</v>
       </c>
@@ -5002,7 +5357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="9" t="s">
         <v>23</v>
       </c>
@@ -5022,7 +5377,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="9" t="s">
         <v>24</v>
       </c>
@@ -5042,7 +5397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="9" t="s">
         <v>25</v>
       </c>
@@ -5062,7 +5417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="9" t="s">
         <v>26</v>
       </c>
@@ -5070,7 +5425,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="9" t="s">
         <v>27</v>
       </c>
@@ -5096,7 +5451,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="9"/>
       <c r="B12" s="17"/>
       <c r="G12" t="s">
@@ -5118,7 +5473,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="15"/>
       <c r="G13" t="s">
         <v>140</v>
@@ -5139,7 +5494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="15"/>
       <c r="G14" t="s">
         <v>448</v>
@@ -5160,7 +5515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
         <v>150</v>
       </c>
@@ -5172,7 +5527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="15"/>
       <c r="G16" t="s">
@@ -5182,7 +5537,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
         <v>152</v>
       </c>
@@ -5201,7 +5556,7 @@
       </c>
       <c r="K17" s="3"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>19</v>
       </c>
@@ -5221,7 +5576,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>20</v>
       </c>
@@ -5241,7 +5596,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>21</v>
       </c>
@@ -5261,7 +5616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>22</v>
       </c>
@@ -5293,7 +5648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>23</v>
       </c>
@@ -5319,7 +5674,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>24</v>
       </c>
@@ -5345,7 +5700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>25</v>
       </c>
@@ -5371,7 +5726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>26</v>
       </c>
@@ -5397,7 +5752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
         <v>27</v>
       </c>
@@ -5423,7 +5778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15">
@@ -5441,7 +5796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="46" t="s">
@@ -5451,12 +5806,12 @@
         <v>379</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="15" t="s">
         <v>152</v>
       </c>
@@ -5464,7 +5819,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="9" t="s">
         <v>19</v>
       </c>
@@ -5472,7 +5827,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="9" t="s">
         <v>20</v>
       </c>
@@ -5483,7 +5838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="9" t="s">
         <v>21</v>
       </c>
@@ -5494,7 +5849,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="9" t="s">
         <v>22</v>
       </c>
@@ -5505,7 +5860,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="9" t="s">
         <v>23</v>
       </c>
@@ -5516,7 +5871,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="9" t="s">
         <v>24</v>
       </c>
@@ -5527,7 +5882,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="9" t="s">
         <v>25</v>
       </c>
@@ -5538,7 +5893,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="9" t="s">
         <v>26</v>
       </c>
@@ -5549,7 +5904,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="9" t="s">
         <v>27</v>
       </c>
@@ -5560,32 +5915,32 @@
         <v>198</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="9"/>
       <c r="B42" s="9"/>
       <c r="E42" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E43" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E44" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="18"/>
     </row>
-    <row r="48" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="37" t="s">
         <v>149</v>
       </c>
@@ -5622,7 +5977,7 @@
       <c r="L48" s="16"/>
       <c r="M48" s="16"/>
     </row>
-    <row r="49" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="39" t="s">
         <v>168</v>
       </c>
@@ -5659,7 +6014,7 @@
       <c r="L49" s="12"/>
       <c r="M49" s="12"/>
     </row>
-    <row r="50" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="39" t="s">
         <v>169</v>
       </c>
@@ -5696,7 +6051,7 @@
       <c r="L50" s="12"/>
       <c r="M50" s="12"/>
     </row>
-    <row r="51" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="39" t="s">
         <v>170</v>
       </c>
@@ -5733,7 +6088,7 @@
       <c r="L51" s="12"/>
       <c r="M51" s="12"/>
     </row>
-    <row r="52" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="39" t="s">
         <v>223</v>
       </c>
@@ -5768,7 +6123,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="39" t="s">
         <v>229</v>
       </c>
@@ -5803,7 +6158,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="39" t="s">
         <v>234</v>
       </c>
@@ -5838,7 +6193,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="39" t="s">
         <v>353</v>
       </c>
@@ -5873,7 +6228,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="39" t="s">
         <v>356</v>
       </c>
@@ -5910,7 +6265,7 @@
       <c r="L56" s="9"/>
       <c r="M56" s="9"/>
     </row>
-    <row r="57" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="39" t="s">
         <v>358</v>
       </c>
@@ -5947,7 +6302,7 @@
       <c r="L57" s="12"/>
       <c r="M57" s="12"/>
     </row>
-    <row r="58" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="39" t="s">
         <v>359</v>
       </c>
@@ -5984,17 +6339,17 @@
       <c r="L58" s="12"/>
       <c r="M58" s="12"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L59" s="12"/>
       <c r="M59" s="12"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" s="41" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="63" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="63" spans="1:13" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="42" t="s">
         <v>179</v>
       </c>
@@ -6026,7 +6381,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="44" t="s">
         <v>168</v>
       </c>
@@ -6058,7 +6413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="44" t="s">
         <v>169</v>
       </c>
@@ -6091,7 +6446,7 @@
       </c>
       <c r="L65" s="9"/>
     </row>
-    <row r="66" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="44" t="s">
         <v>170</v>
       </c>
@@ -6124,7 +6479,7 @@
       </c>
       <c r="L66" s="9"/>
     </row>
-    <row r="67" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="44" t="s">
         <v>223</v>
       </c>
@@ -6158,7 +6513,7 @@
       <c r="K67" s="9"/>
       <c r="L67" s="9"/>
     </row>
-    <row r="68" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="44" t="s">
         <v>229</v>
       </c>
@@ -6192,7 +6547,7 @@
       <c r="K68" s="9"/>
       <c r="L68" s="9"/>
     </row>
-    <row r="69" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="44" t="s">
         <v>234</v>
       </c>
@@ -6226,7 +6581,7 @@
       <c r="K69" s="9"/>
       <c r="L69" s="9"/>
     </row>
-    <row r="70" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="44" t="s">
         <v>353</v>
       </c>
@@ -6260,7 +6615,7 @@
       <c r="K70" s="9"/>
       <c r="L70" s="9"/>
     </row>
-    <row r="71" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="44" t="s">
         <v>356</v>
       </c>
@@ -6294,7 +6649,7 @@
       <c r="K71" s="9"/>
       <c r="L71" s="9"/>
     </row>
-    <row r="72" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72" s="44" t="s">
         <v>358</v>
       </c>
@@ -6328,7 +6683,7 @@
       <c r="K72" s="9"/>
       <c r="L72" s="9"/>
     </row>
-    <row r="73" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="44" t="s">
         <v>359</v>
       </c>
@@ -6362,12 +6717,12 @@
       <c r="K73" s="9"/>
       <c r="L73" s="9"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="18" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>184</v>
       </c>
@@ -6378,7 +6733,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>168</v>
       </c>
@@ -6401,7 +6756,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>169</v>
       </c>
@@ -6424,7 +6779,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>170</v>
       </c>
@@ -6447,7 +6802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>223</v>
       </c>
@@ -6470,7 +6825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>229</v>
       </c>
@@ -6493,7 +6848,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>234</v>
       </c>
@@ -6516,7 +6871,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>353</v>
       </c>
@@ -6539,7 +6894,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>356</v>
       </c>
@@ -6562,7 +6917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>358</v>
       </c>
@@ -6585,7 +6940,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>359</v>
       </c>
@@ -6608,7 +6963,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>270</v>
       </c>
@@ -6619,7 +6974,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>168</v>
       </c>
@@ -6642,7 +6997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>169</v>
       </c>
@@ -6665,7 +7020,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>170</v>
       </c>
@@ -6688,7 +7043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>223</v>
       </c>
@@ -6711,7 +7066,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>229</v>
       </c>
@@ -6734,7 +7089,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>234</v>
       </c>
@@ -6757,7 +7112,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>353</v>
       </c>
@@ -6780,7 +7135,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>356</v>
       </c>
@@ -6803,7 +7158,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>358</v>
       </c>
@@ -6826,7 +7181,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>359</v>
       </c>
@@ -6849,7 +7204,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>190</v>
       </c>
@@ -6860,7 +7215,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>168</v>
       </c>
@@ -6883,7 +7238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>169</v>
       </c>
@@ -6906,7 +7261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>170</v>
       </c>
@@ -6929,7 +7284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>223</v>
       </c>
@@ -6952,7 +7307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>229</v>
       </c>
@@ -6975,7 +7330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>234</v>
       </c>
@@ -6998,7 +7353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>353</v>
       </c>
@@ -7021,7 +7376,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>356</v>
       </c>
@@ -7044,7 +7399,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>358</v>
       </c>
@@ -7067,7 +7422,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>359</v>
       </c>
@@ -7090,12 +7445,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A117" s="9" t="s">
         <v>179</v>
       </c>
@@ -7128,7 +7483,7 @@
       </c>
       <c r="L117" s="9"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A118" s="9" t="s">
         <v>168</v>
       </c>
@@ -7170,7 +7525,7 @@
       </c>
       <c r="L118" s="20"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A119" s="9" t="s">
         <v>169</v>
       </c>
@@ -7212,7 +7567,7 @@
       </c>
       <c r="L119" s="20"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A120" s="9" t="s">
         <v>170</v>
       </c>
@@ -7254,7 +7609,7 @@
       </c>
       <c r="L120" s="9"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="s">
         <v>223</v>
       </c>
@@ -7296,7 +7651,7 @@
       </c>
       <c r="L121" s="9"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
         <v>229</v>
       </c>
@@ -7338,7 +7693,7 @@
       </c>
       <c r="L122" s="9"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
         <v>234</v>
       </c>
@@ -7380,7 +7735,7 @@
       </c>
       <c r="L123" s="9"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="s">
         <v>353</v>
       </c>
@@ -7421,7 +7776,7 @@
       </c>
       <c r="L124" s="9"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A125" s="4" t="s">
         <v>356</v>
       </c>
@@ -7463,7 +7818,7 @@
       </c>
       <c r="L125" s="9"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
         <v>358</v>
       </c>
@@ -7505,7 +7860,7 @@
       </c>
       <c r="L126" s="9"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="s">
         <v>359</v>
       </c>
@@ -7546,7 +7901,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>195</v>
       </c>
@@ -7554,7 +7909,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A132" s="9" t="s">
         <v>179</v>
       </c>
@@ -7592,7 +7947,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A133" s="9" t="s">
         <v>168</v>
       </c>
@@ -7644,7 +7999,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A134" s="9" t="s">
         <v>169</v>
       </c>
@@ -7696,7 +8051,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A135" s="9" t="s">
         <v>170</v>
       </c>
@@ -7748,7 +8103,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="s">
         <v>223</v>
       </c>
@@ -7800,7 +8155,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="s">
         <v>229</v>
       </c>
@@ -7849,7 +8204,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A138" s="4" t="s">
         <v>234</v>
       </c>
@@ -7898,7 +8253,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A139" s="4" t="s">
         <v>353</v>
       </c>
@@ -7950,7 +8305,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A140" s="4" t="s">
         <v>356</v>
       </c>
@@ -8002,7 +8357,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A141" s="4" t="s">
         <v>358</v>
       </c>
@@ -8054,7 +8409,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A142" s="4" t="s">
         <v>359</v>
       </c>
@@ -8130,28 +8485,28 @@
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
-    <col min="3" max="5" width="13.21875" customWidth="1"/>
-    <col min="6" max="8" width="20.44140625" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.6328125" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="3" max="5" width="13.1796875" customWidth="1"/>
+    <col min="6" max="8" width="20.453125" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" customWidth="1"/>
+    <col min="10" max="10" width="17.6328125" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" customWidth="1"/>
-    <col min="14" max="14" width="14.44140625" customWidth="1"/>
-    <col min="15" max="15" width="15.77734375" customWidth="1"/>
+    <col min="12" max="12" width="10.54296875" customWidth="1"/>
+    <col min="13" max="13" width="11.08984375" customWidth="1"/>
+    <col min="14" max="14" width="14.453125" customWidth="1"/>
+    <col min="15" max="15" width="15.81640625" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
-    <col min="17" max="17" width="11.44140625" customWidth="1"/>
-    <col min="18" max="18" width="18.44140625" customWidth="1"/>
-    <col min="19" max="19" width="22.21875" customWidth="1"/>
-    <col min="20" max="20" width="33.109375" customWidth="1"/>
-    <col min="24" max="24" width="17.44140625" customWidth="1"/>
+    <col min="17" max="17" width="11.453125" customWidth="1"/>
+    <col min="18" max="18" width="18.453125" customWidth="1"/>
+    <col min="19" max="19" width="22.1796875" customWidth="1"/>
+    <col min="20" max="20" width="33.08984375" customWidth="1"/>
+    <col min="24" max="24" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>151</v>
       </c>
@@ -8159,7 +8514,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>152</v>
       </c>
@@ -8167,7 +8522,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>19</v>
       </c>
@@ -8193,7 +8548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>20</v>
       </c>
@@ -8222,7 +8577,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>21</v>
       </c>
@@ -8251,7 +8606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>22</v>
       </c>
@@ -8280,7 +8635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>23</v>
       </c>
@@ -8309,7 +8664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>24</v>
       </c>
@@ -8338,7 +8693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>25</v>
       </c>
@@ -8346,7 +8701,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>26</v>
       </c>
@@ -8354,7 +8709,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>27</v>
       </c>
@@ -8380,7 +8735,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
       <c r="B12" s="17"/>
       <c r="J12" t="s">
@@ -8402,7 +8757,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B13" s="15"/>
       <c r="J13" t="s">
         <v>241</v>
@@ -8423,7 +8778,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B14" s="15"/>
       <c r="J14" t="s">
         <v>242</v>
@@ -8444,7 +8799,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
         <v>150</v>
       </c>
@@ -8462,7 +8817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="15"/>
       <c r="J16" t="s">
@@ -8478,7 +8833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
         <v>152</v>
       </c>
@@ -8500,7 +8855,7 @@
       <c r="G17" s="9"/>
       <c r="O17" s="3"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>19</v>
       </c>
@@ -8532,7 +8887,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>20</v>
       </c>
@@ -8564,7 +8919,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>21</v>
       </c>
@@ -8596,7 +8951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>22</v>
       </c>
@@ -8640,7 +8995,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>23</v>
       </c>
@@ -8687,7 +9042,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>24</v>
       </c>
@@ -8728,7 +9083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>25</v>
       </c>
@@ -8769,7 +9124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>26</v>
       </c>
@@ -8810,7 +9165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
         <v>27</v>
       </c>
@@ -8851,7 +9206,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17">
@@ -8873,19 +9228,19 @@
       <c r="G27" s="9"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
         <v>152</v>
       </c>
@@ -8913,7 +9268,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
         <v>19</v>
       </c>
@@ -8943,7 +9298,7 @@
         <v>31.432980599647259</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>20</v>
       </c>
@@ -8973,7 +9328,7 @@
         <v>20.321869488536155</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
         <v>21</v>
       </c>
@@ -9003,7 +9358,7 @@
         <v>14.766313932980598</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
         <v>22</v>
       </c>
@@ -9033,7 +9388,7 @@
         <v>11.062610229276896</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
         <v>23</v>
       </c>
@@ -9063,7 +9418,7 @@
         <v>8.284832451499117</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
         <v>24</v>
       </c>
@@ -9095,7 +9450,7 @@
       <c r="R38" s="3"/>
       <c r="S38" s="3"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
         <v>25</v>
       </c>
@@ -9127,7 +9482,7 @@
       <c r="R39" s="3"/>
       <c r="S39" s="3"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
         <v>26</v>
       </c>
@@ -9159,7 +9514,7 @@
       <c r="R40" s="3"/>
       <c r="S40" s="3"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
         <v>27</v>
       </c>
@@ -9189,7 +9544,7 @@
         <v>1.2345679012345678</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A42" s="9"/>
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
@@ -9210,15 +9565,15 @@
         <v>99.999999999999986</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A47" s="18"/>
     </row>
-    <row r="48" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="16" t="s">
         <v>77</v>
       </c>
@@ -9259,7 +9614,7 @@
       <c r="P48" s="16"/>
       <c r="Q48" s="16"/>
     </row>
-    <row r="49" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A49" s="16" t="s">
         <v>168</v>
       </c>
@@ -9300,7 +9655,7 @@
       <c r="P49" s="12"/>
       <c r="Q49" s="12"/>
     </row>
-    <row r="50" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A50" s="16" t="s">
         <v>169</v>
       </c>
@@ -9341,7 +9696,7 @@
       <c r="P50" s="12"/>
       <c r="Q50" s="12"/>
     </row>
-    <row r="51" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A51" s="16" t="s">
         <v>170</v>
       </c>
@@ -9382,7 +9737,7 @@
       <c r="P51" s="12"/>
       <c r="Q51" s="12"/>
     </row>
-    <row r="52" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A52" s="16" t="s">
         <v>223</v>
       </c>
@@ -9421,7 +9776,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" s="16" t="s">
         <v>229</v>
       </c>
@@ -9460,7 +9815,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="16" t="s">
         <v>234</v>
       </c>
@@ -9499,7 +9854,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
         <v>149</v>
       </c>
@@ -9540,7 +9895,7 @@
       <c r="Q56" s="9"/>
       <c r="R56" s="9"/>
     </row>
-    <row r="57" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
         <v>168</v>
       </c>
@@ -9581,7 +9936,7 @@
       <c r="Q57" s="9"/>
       <c r="R57" s="17"/>
     </row>
-    <row r="58" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
         <v>169</v>
       </c>
@@ -9622,7 +9977,7 @@
       <c r="Q58" s="9"/>
       <c r="R58" s="17"/>
     </row>
-    <row r="59" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
         <v>170</v>
       </c>
@@ -9663,7 +10018,7 @@
       <c r="Q59" s="9"/>
       <c r="R59" s="17"/>
     </row>
-    <row r="60" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A60" s="9" t="s">
         <v>223</v>
       </c>
@@ -9704,7 +10059,7 @@
       <c r="Q60" s="9"/>
       <c r="R60" s="17"/>
     </row>
-    <row r="61" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
         <v>229</v>
       </c>
@@ -9745,7 +10100,7 @@
       <c r="Q61" s="9"/>
       <c r="R61" s="17"/>
     </row>
-    <row r="62" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
         <v>234</v>
       </c>
@@ -9786,22 +10141,22 @@
       <c r="Q62" s="9"/>
       <c r="R62" s="17"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="Q63" s="9"/>
       <c r="R63" s="17"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>178</v>
       </c>
       <c r="Q64" s="9"/>
       <c r="R64" s="17"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="Q65" s="9"/>
       <c r="R65" s="17"/>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
         <v>179</v>
       </c>
@@ -9838,7 +10193,7 @@
       </c>
       <c r="O66" s="9"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A67" s="9" t="s">
         <v>168</v>
       </c>
@@ -9875,7 +10230,7 @@
       </c>
       <c r="O67" s="9"/>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A68" s="9" t="s">
         <v>169</v>
       </c>
@@ -9912,7 +10267,7 @@
       </c>
       <c r="O68" s="9"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A69" s="9" t="s">
         <v>170</v>
       </c>
@@ -9949,7 +10304,7 @@
       </c>
       <c r="O69" s="9"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A70" s="9" t="s">
         <v>223</v>
       </c>
@@ -9986,7 +10341,7 @@
       </c>
       <c r="O70" s="9"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A71" s="9" t="s">
         <v>229</v>
       </c>
@@ -10023,7 +10378,7 @@
       </c>
       <c r="O71" s="9"/>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
         <v>234</v>
       </c>
@@ -10060,15 +10415,15 @@
       </c>
       <c r="O72" s="9"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
       <c r="N73" s="9"/>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A74" s="18" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>184</v>
       </c>
@@ -10079,7 +10434,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>168</v>
       </c>
@@ -10102,7 +10457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>169</v>
       </c>
@@ -10125,7 +10480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>170</v>
       </c>
@@ -10148,7 +10503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>223</v>
       </c>
@@ -10171,7 +10526,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>229</v>
       </c>
@@ -10194,7 +10549,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>234</v>
       </c>
@@ -10217,7 +10572,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>270</v>
       </c>
@@ -10228,7 +10583,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>168</v>
       </c>
@@ -10251,7 +10606,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>169</v>
       </c>
@@ -10274,7 +10629,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>170</v>
       </c>
@@ -10297,7 +10652,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>223</v>
       </c>
@@ -10320,7 +10675,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>229</v>
       </c>
@@ -10343,7 +10698,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>234</v>
       </c>
@@ -10366,7 +10721,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>267</v>
       </c>
@@ -10377,7 +10732,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>168</v>
       </c>
@@ -10401,7 +10756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>169</v>
       </c>
@@ -10425,7 +10780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>170</v>
       </c>
@@ -10448,7 +10803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>223</v>
       </c>
@@ -10471,7 +10826,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>229</v>
       </c>
@@ -10494,7 +10849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>234</v>
       </c>
@@ -10517,16 +10872,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
       <c r="J100" s="19"/>
       <c r="O100" s="19"/>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A103" s="9" t="s">
         <v>179</v>
       </c>
@@ -10563,7 +10918,7 @@
       </c>
       <c r="P103" s="9"/>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A104" s="9" t="s">
         <v>168</v>
       </c>
@@ -10609,7 +10964,7 @@
       </c>
       <c r="P104" s="20"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A105" s="9" t="s">
         <v>169</v>
       </c>
@@ -10655,7 +11010,7 @@
       </c>
       <c r="P105" s="20"/>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A106" s="9" t="s">
         <v>170</v>
       </c>
@@ -10701,7 +11056,7 @@
       </c>
       <c r="P106" s="9"/>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A107" s="9" t="s">
         <v>223</v>
       </c>
@@ -10748,7 +11103,7 @@
       <c r="O107" s="9"/>
       <c r="P107" s="9"/>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A108" s="9" t="s">
         <v>229</v>
       </c>
@@ -10793,7 +11148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A109" s="9" t="s">
         <v>234</v>
       </c>
@@ -10838,12 +11193,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A113" s="9" t="s">
         <v>179</v>
       </c>
@@ -10885,7 +11240,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A114" s="9" t="s">
         <v>168</v>
       </c>
@@ -10938,7 +11293,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A115" s="9" t="s">
         <v>169</v>
       </c>
@@ -10991,7 +11346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A116" s="9" t="s">
         <v>170</v>
       </c>
@@ -11044,7 +11399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A117" s="9" t="s">
         <v>223</v>
       </c>
@@ -11098,7 +11453,7 @@
       </c>
       <c r="R117" s="9"/>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A118" s="9" t="s">
         <v>229</v>
       </c>
@@ -11151,7 +11506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A119" s="9" t="s">
         <v>234</v>
       </c>
@@ -11225,24 +11580,24 @@
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="27.44140625" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" customWidth="1"/>
-    <col min="10" max="10" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.6328125" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" customWidth="1"/>
+    <col min="6" max="6" width="27.453125" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" customWidth="1"/>
+    <col min="8" max="8" width="11.08984375" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" customWidth="1"/>
+    <col min="10" max="10" width="15.81640625" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" customWidth="1"/>
-    <col min="14" max="14" width="20.21875" customWidth="1"/>
-    <col min="18" max="18" width="17.44140625" customWidth="1"/>
+    <col min="12" max="12" width="11.453125" customWidth="1"/>
+    <col min="14" max="14" width="20.1796875" customWidth="1"/>
+    <col min="18" max="18" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>151</v>
       </c>
@@ -11253,12 +11608,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="U2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>19</v>
       </c>
@@ -11287,7 +11642,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>20</v>
       </c>
@@ -11316,7 +11671,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>21</v>
       </c>
@@ -11345,7 +11700,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>22</v>
       </c>
@@ -11374,7 +11729,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>23</v>
       </c>
@@ -11394,7 +11749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>24</v>
       </c>
@@ -11417,7 +11772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>25</v>
       </c>
@@ -11440,7 +11795,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>26</v>
       </c>
@@ -11451,7 +11806,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>27</v>
       </c>
@@ -11480,7 +11835,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
       <c r="B12" s="17"/>
       <c r="F12" t="s">
@@ -11505,7 +11860,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B13" s="15"/>
       <c r="F13" t="s">
         <v>140</v>
@@ -11529,7 +11884,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B14" s="15"/>
       <c r="F14" t="s">
         <v>180</v>
@@ -11553,7 +11908,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
         <v>150</v>
       </c>
@@ -11574,7 +11929,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="15"/>
       <c r="F16" t="s">
@@ -11593,7 +11948,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
         <v>152</v>
       </c>
@@ -11619,7 +11974,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>19</v>
       </c>
@@ -11640,7 +11995,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>20</v>
       </c>
@@ -11658,7 +12013,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>21</v>
       </c>
@@ -11676,7 +12031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>22</v>
       </c>
@@ -11706,7 +12061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>23</v>
       </c>
@@ -11730,7 +12085,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>24</v>
       </c>
@@ -11754,7 +12109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>25</v>
       </c>
@@ -11778,7 +12133,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>26</v>
       </c>
@@ -11802,7 +12157,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
         <v>27</v>
       </c>
@@ -11826,7 +12181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="B27" s="15"/>
       <c r="C27" s="30">
@@ -11846,17 +12201,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
         <v>152</v>
       </c>
@@ -11864,7 +12219,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
         <v>19</v>
       </c>
@@ -11872,7 +12227,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>20</v>
       </c>
@@ -11880,7 +12235,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
         <v>21</v>
       </c>
@@ -11888,7 +12243,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
         <v>22</v>
       </c>
@@ -11896,7 +12251,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
         <v>23</v>
       </c>
@@ -11904,7 +12259,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
         <v>24</v>
       </c>
@@ -11912,7 +12267,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
         <v>25</v>
       </c>
@@ -11920,7 +12275,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
         <v>26</v>
       </c>
@@ -11928,7 +12283,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
         <v>27</v>
       </c>
@@ -11936,7 +12291,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
         <v>28</v>
       </c>
@@ -11944,15 +12299,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="18"/>
     </row>
-    <row r="48" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="16" t="s">
         <v>77</v>
       </c>
@@ -11990,7 +12345,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="12">
         <v>1</v>
       </c>
@@ -12006,7 +12361,7 @@
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="12">
         <v>2</v>
       </c>
@@ -12022,7 +12377,7 @@
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="12">
         <v>3</v>
       </c>
@@ -12038,12 +12393,12 @@
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
         <v>149</v>
       </c>
@@ -12081,7 +12436,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
         <v>168</v>
       </c>
@@ -12097,7 +12452,7 @@
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
         <v>169</v>
       </c>
@@ -12113,7 +12468,7 @@
       <c r="K58" s="12"/>
       <c r="L58" s="12"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
         <v>170</v>
       </c>
@@ -12129,12 +12484,12 @@
       <c r="K59" s="12"/>
       <c r="L59" s="12"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" s="9" t="s">
         <v>179</v>
       </c>
@@ -12169,7 +12524,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
         <v>168</v>
       </c>
@@ -12184,7 +12539,7 @@
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" s="9" t="s">
         <v>169</v>
       </c>
@@ -12199,7 +12554,7 @@
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" s="9" t="s">
         <v>170</v>
       </c>
@@ -12214,12 +12569,12 @@
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="18" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>184</v>
       </c>
@@ -12230,7 +12585,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>168</v>
       </c>
@@ -12253,7 +12608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>169</v>
       </c>
@@ -12276,7 +12631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>170</v>
       </c>
@@ -12299,7 +12654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>187</v>
       </c>
@@ -12310,7 +12665,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>168</v>
       </c>
@@ -12333,7 +12688,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>169</v>
       </c>
@@ -12356,7 +12711,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>170</v>
       </c>
@@ -12379,7 +12734,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>190</v>
       </c>
@@ -12390,7 +12745,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>168</v>
       </c>
@@ -12413,7 +12768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>169</v>
       </c>
@@ -12436,7 +12791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>170</v>
       </c>
@@ -12459,12 +12814,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E91" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E92" t="s">
         <v>168</v>
       </c>
@@ -12473,7 +12828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E93" t="s">
         <v>169</v>
       </c>
@@ -12482,7 +12837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E94" t="s">
         <v>170</v>
       </c>
@@ -12491,12 +12846,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" s="9" t="s">
         <v>179</v>
       </c>
@@ -12531,7 +12886,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" s="9" t="s">
         <v>168</v>
       </c>
@@ -12576,7 +12931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A102" s="9" t="s">
         <v>169</v>
       </c>
@@ -12621,7 +12976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A103" s="9" t="s">
         <v>170</v>
       </c>
@@ -12666,12 +13021,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A109" s="9" t="s">
         <v>179</v>
       </c>
@@ -12712,7 +13067,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A110" s="9" t="s">
         <v>168</v>
       </c>
@@ -12765,7 +13120,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A111" s="9" t="s">
         <v>169</v>
       </c>
@@ -12818,7 +13173,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A112" s="9" t="s">
         <v>170</v>
       </c>
@@ -12890,14 +13245,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
-    <col min="2" max="2" width="21.21875" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" customWidth="1"/>
+    <col min="1" max="1" width="20.08984375" customWidth="1"/>
+    <col min="2" max="2" width="21.1796875" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>285</v>
       </c>
@@ -12908,7 +13263,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>287</v>
       </c>
@@ -12919,7 +13274,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>288</v>
       </c>
@@ -12930,7 +13285,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>289</v>
       </c>
@@ -12938,7 +13293,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>290</v>
       </c>
@@ -12946,7 +13301,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>291</v>
       </c>
@@ -12954,7 +13309,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>292</v>
       </c>
@@ -12962,7 +13317,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>293</v>
       </c>
@@ -12970,7 +13325,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>294</v>
       </c>
@@ -12991,15 +13346,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" customWidth="1"/>
-    <col min="10" max="10" width="18.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="4" max="4" width="19.90625" customWidth="1"/>
+    <col min="7" max="7" width="18.08984375" customWidth="1"/>
+    <col min="10" max="10" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -13010,7 +13365,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -13022,7 +13377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -13034,7 +13389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -13046,7 +13401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -13058,7 +13413,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -13070,7 +13425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -13082,7 +13437,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -13094,7 +13449,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -13106,7 +13461,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -13118,7 +13473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -13130,13 +13485,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B12">
         <f>SUM(B2:B11)</f>
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -13150,7 +13505,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -13182,7 +13537,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -13214,7 +13569,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -13246,7 +13601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -13278,7 +13633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -13310,7 +13665,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -13342,7 +13697,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -13374,7 +13729,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -13406,7 +13761,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -13438,7 +13793,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -13470,7 +13825,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -13502,7 +13857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B25">
         <f>SUM(B15:B24)</f>
         <v>100</v>

</xml_diff>